<commit_message>
Up charging current to 6A
</commit_message>
<xml_diff>
--- a/Design/bqstroller calculation tools_V1.5.xlsx
+++ b/Design/bqstroller calculation tools_V1.5.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tachi\Documents\Nerd Shit\rm_electrical-supercap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tachi\Documents\Nerd Shit\rm_electrical-supercap\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE3542D-E556-4EF3-9C6A-CB958D04A7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E6D17C-8174-424F-B324-0312CCF28FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="877" activeTab="6" xr2:uid="{A7C7322A-F6CE-4642-9509-D11806E70597}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="877" activeTab="6" xr2:uid="{A7C7322A-F6CE-4642-9509-D11806E70597}"/>
   </bookViews>
   <sheets>
     <sheet name="bq24600" sheetId="31" r:id="rId1"/>
@@ -1031,13 +1031,13 @@
     <t>NO precharge, NO termination</t>
   </si>
   <si>
-    <t>220k//68k</t>
+    <t>47k</t>
   </si>
   <si>
-    <t>39k</t>
+    <t>390k//47k</t>
   </si>
   <si>
-    <t>47k</t>
+    <t>68k</t>
   </si>
 </sst>
 </file>
@@ -10661,6 +10661,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B46:D46"/>
     <mergeCell ref="B94:D94"/>
     <mergeCell ref="B79:D79"/>
     <mergeCell ref="B76:D76"/>
@@ -10668,12 +10674,6 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B71:D71"/>
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B46:D46"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11760,6 +11760,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B94:D94"/>
     <mergeCell ref="F74:H74"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B79:D79"/>
@@ -11768,11 +11773,6 @@
     <mergeCell ref="B54:D54"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B94:D94"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12876,6 +12876,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B94:D94"/>
     <mergeCell ref="F74:H74"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B79:D79"/>
@@ -12884,11 +12889,6 @@
     <mergeCell ref="B54:D54"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B94:D94"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14041,7 +14041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D25B887-5317-4EE6-BF4D-6ADB0AAD2CC1}">
   <dimension ref="B1:K95"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
@@ -14805,6 +14805,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B94:D94"/>
     <mergeCell ref="F74:H74"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B79:D79"/>
@@ -14813,11 +14818,6 @@
     <mergeCell ref="B54:D54"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B94:D94"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15134,7 +15134,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0B0618-A931-4BD7-89EE-A2BDD74EB831}">
   <dimension ref="B1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" workbookViewId="0">
       <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
@@ -15212,7 +15212,7 @@
         <v>143</v>
       </c>
       <c r="C27" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>144</v>
@@ -15223,7 +15223,7 @@
         <v>145</v>
       </c>
       <c r="C28" s="37">
-        <v>4</v>
+        <v>2.7</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>146</v>
@@ -15235,7 +15235,7 @@
       </c>
       <c r="C29" s="15">
         <f>C27*C28</f>
-        <v>4</v>
+        <v>5.4</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>1</v>
@@ -15246,13 +15246,14 @@
         <v>30</v>
       </c>
       <c r="C30" s="41">
-        <v>51.944400000000002</v>
+        <f>1/(1/390+1/47)</f>
+        <v>41.945080091533178</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>7</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G30" s="82"/>
     </row>
@@ -15262,7 +15263,7 @@
       </c>
       <c r="C31" s="15">
         <f>(C29-2.1)/2.1*C30</f>
-        <v>46.997314285714282</v>
+        <v>65.913697286694998</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>0</v>
@@ -15288,7 +15289,7 @@
         <v>11</v>
       </c>
       <c r="C34" s="37">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>12</v>
@@ -15325,7 +15326,7 @@
       </c>
       <c r="C37" s="15">
         <f>20*C35*C34/1000</f>
-        <v>0.8</v>
+        <v>1.2</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>6</v>
@@ -15336,7 +15337,7 @@
         <v>37</v>
       </c>
       <c r="C38" s="42">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>7</v>
@@ -15348,13 +15349,13 @@
       </c>
       <c r="C39" s="16">
         <f>C38/((C36/C37)-1)</f>
-        <v>38.400000000000013</v>
+        <v>46.857142857142854</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>15</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="2:11">
@@ -15402,7 +15403,7 @@
       </c>
       <c r="C43" s="15">
         <f>C29</f>
-        <v>4</v>
+        <v>5.4</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>17</v>
@@ -15432,7 +15433,7 @@
       </c>
       <c r="C44" s="45">
         <f>C43/C42</f>
-        <v>0.16666666666666666</v>
+        <v>0.22500000000000001</v>
       </c>
       <c r="D44" s="4"/>
       <c r="F44" s="20" t="s">
@@ -15488,7 +15489,7 @@
         <v>18</v>
       </c>
       <c r="C46" s="43">
-        <v>6.8</v>
+        <v>4.7</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>120</v>
@@ -15500,7 +15501,7 @@
       </c>
       <c r="C47" s="16">
         <f>1000*(C42-C43)*C44/C46/C45</f>
-        <v>0.81699346405228757</v>
+        <v>1.4840425531914894</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>21</v>
@@ -15512,7 +15513,7 @@
       </c>
       <c r="C48" s="16">
         <f>1000*1000000*(C43-C43*C43/C42)/(8*C51*C52*C45*C45)</f>
-        <v>6.8404693109184835</v>
+        <v>12.517228012748731</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>105</v>
@@ -15535,8 +15536,8 @@
         <v>22</v>
       </c>
       <c r="C51" s="44">
-        <f>4.7*1.2</f>
-        <v>5.64</v>
+        <f>C46</f>
+        <v>4.7</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>120</v>
@@ -15547,7 +15548,7 @@
         <v>24</v>
       </c>
       <c r="C52" s="44">
-        <v>30</v>
+        <v>24.7</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>121</v>
@@ -15559,7 +15560,7 @@
       </c>
       <c r="C53" s="16">
         <f>1000/(SQRT(C51*C52))/2/PI()</f>
-        <v>12.23545015952789</v>
+        <v>14.771436302483211</v>
       </c>
       <c r="D53" s="4" t="s">
         <v>26</v>
@@ -15705,15 +15706,15 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B33:D33"/>
     <mergeCell ref="B69:D69"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B50:D50"/>
     <mergeCell ref="F53:H53"/>
     <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B33:D33"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15955,7 +15956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2E1798A-6386-45B9-A307-7C5A5BAA18E0}">
   <dimension ref="B1:J72"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="90" workbookViewId="0">
+    <sheetView zoomScale="90" workbookViewId="0">
       <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
@@ -16528,6 +16529,9 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="F59:H59"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B17:D17"/>
     <mergeCell ref="B71:D71"/>
     <mergeCell ref="B27:D27"/>
     <mergeCell ref="B33:D33"/>
@@ -16536,9 +16540,6 @@
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="B61:D61"/>
     <mergeCell ref="B38:D38"/>
-    <mergeCell ref="F59:H59"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B17:D17"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updating buck converter to work with new 2S2P supercap stackup
</commit_message>
<xml_diff>
--- a/Design/bqstroller calculation tools_V1.5.xlsx
+++ b/Design/bqstroller calculation tools_V1.5.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tachi\Documents\Nerd Shit\rm_electrical-supercap\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81E6D17C-8174-424F-B324-0312CCF28FDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C65BDF-DFA8-4070-95AB-2213AFEDEA1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" tabRatio="877" activeTab="6" xr2:uid="{A7C7322A-F6CE-4642-9509-D11806E70597}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="877" activeTab="6" xr2:uid="{A7C7322A-F6CE-4642-9509-D11806E70597}"/>
   </bookViews>
   <sheets>
     <sheet name="bq24600" sheetId="31" r:id="rId1"/>
@@ -1034,10 +1034,10 @@
     <t>47k</t>
   </si>
   <si>
-    <t>390k//47k</t>
+    <t>470k//15k</t>
   </si>
   <si>
-    <t>68k</t>
+    <t>27k</t>
   </si>
 </sst>
 </file>
@@ -10661,12 +10661,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="F74:H74"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B53:D53"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B46:D46"/>
     <mergeCell ref="B94:D94"/>
     <mergeCell ref="B79:D79"/>
     <mergeCell ref="B76:D76"/>
@@ -10674,6 +10668,12 @@
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B38:D38"/>
     <mergeCell ref="B71:D71"/>
+    <mergeCell ref="F74:H74"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B53:D53"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B46:D46"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -11760,11 +11760,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B94:D94"/>
     <mergeCell ref="F74:H74"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B79:D79"/>
@@ -11773,6 +11768,11 @@
     <mergeCell ref="B54:D54"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B94:D94"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12876,11 +12876,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B94:D94"/>
     <mergeCell ref="F74:H74"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B79:D79"/>
@@ -12889,6 +12884,11 @@
     <mergeCell ref="B54:D54"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B94:D94"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14805,11 +14805,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B94:D94"/>
     <mergeCell ref="F74:H74"/>
     <mergeCell ref="B76:D76"/>
     <mergeCell ref="B79:D79"/>
@@ -14818,6 +14813,11 @@
     <mergeCell ref="B54:D54"/>
     <mergeCell ref="B62:D62"/>
     <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B94:D94"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -15134,8 +15134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0B0618-A931-4BD7-89EE-A2BDD74EB831}">
   <dimension ref="B1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="90" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75"/>
@@ -15223,7 +15223,7 @@
         <v>145</v>
       </c>
       <c r="C28" s="37">
-        <v>2.7</v>
+        <v>3</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>146</v>
@@ -15235,7 +15235,7 @@
       </c>
       <c r="C29" s="15">
         <f>C27*C28</f>
-        <v>5.4</v>
+        <v>6</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>1</v>
@@ -15246,8 +15246,8 @@
         <v>30</v>
       </c>
       <c r="C30" s="41">
-        <f>1/(1/390+1/47)</f>
-        <v>41.945080091533178</v>
+        <f>1/(1/470+1/15)</f>
+        <v>14.536082474226804</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>7</v>
@@ -15263,7 +15263,7 @@
       </c>
       <c r="C31" s="15">
         <f>(C29-2.1)/2.1*C30</f>
-        <v>65.913697286694998</v>
+        <v>26.995581737849776</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>0</v>
@@ -15403,7 +15403,7 @@
       </c>
       <c r="C43" s="15">
         <f>C29</f>
-        <v>5.4</v>
+        <v>6</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>17</v>
@@ -15433,7 +15433,7 @@
       </c>
       <c r="C44" s="45">
         <f>C43/C42</f>
-        <v>0.22500000000000001</v>
+        <v>0.25</v>
       </c>
       <c r="D44" s="4"/>
       <c r="F44" s="20" t="s">
@@ -15501,7 +15501,7 @@
       </c>
       <c r="C47" s="16">
         <f>1000*(C42-C43)*C44/C46/C45</f>
-        <v>1.4840425531914894</v>
+        <v>1.5957446808510638</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>21</v>
@@ -15513,7 +15513,7 @@
       </c>
       <c r="C48" s="16">
         <f>1000*1000000*(C43-C43*C43/C42)/(8*C51*C52*C45*C45)</f>
-        <v>12.517228012748731</v>
+        <v>13.45938495994487</v>
       </c>
       <c r="D48" s="4" t="s">
         <v>105</v>
@@ -15706,6 +15706,8 @@
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="F53:H53"/>
+    <mergeCell ref="B59:D59"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B32:D32"/>
@@ -15713,8 +15715,6 @@
     <mergeCell ref="B69:D69"/>
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B50:D50"/>
-    <mergeCell ref="F53:H53"/>
-    <mergeCell ref="B59:D59"/>
   </mergeCells>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>